<commit_message>
Adding a little more complexity to sample sheet
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\temp\excelconversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535C5FC7-1252-4D30-95E7-B466403EDA9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB55D8F3-57A2-42F0-8EB3-F59AE737B447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4560" yWindow="4560" windowWidth="28800" windowHeight="15290" xr2:uid="{84ABE200-A998-41AD-B65F-26DE3D1D25B2}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="15105" activeTab="1" xr2:uid="{84ABE200-A998-41AD-B65F-26DE3D1D25B2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Base" sheetId="1" r:id="rId1"/>
+    <sheet name="Range" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Min værdi</t>
   </si>
@@ -70,17 +70,26 @@
     <t>Fra sheet 2</t>
   </si>
   <si>
-    <t>My Range</t>
-  </si>
-  <si>
     <t>Sum from Sheet 3</t>
+  </si>
+  <si>
+    <t>Tax rate</t>
+  </si>
+  <si>
+    <t>Applied Tax</t>
+  </si>
+  <si>
+    <t>Number range</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,16 +97,44 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -105,17 +142,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -126,6 +181,20 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6BCC2F25-AABA-4611-8FD5-91B834D307C1}" name="Table1" displayName="Table1" ref="A1:C12" totalsRowShown="0" headerRowCellStyle="Normal">
+  <autoFilter ref="A1:C12" xr:uid="{6BCC2F25-AABA-4611-8FD5-91B834D307C1}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{A62FA880-DA89-4C09-885B-61D26E065F1B}" name="Number range"/>
+    <tableColumn id="2" xr3:uid="{C905EB97-73C3-4F24-9614-B038CF69D6E6}" name="Applied Tax"/>
+    <tableColumn id="3" xr3:uid="{510D38E0-FA25-4BCD-B487-7411F8EA7C20}" name="Total" dataDxfId="0">
+      <calculatedColumnFormula>A2+B2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -447,16 +516,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A3C5551-7AC7-47CF-9FAB-6AC729A5F45A}">
   <dimension ref="A4:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -464,7 +533,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -472,7 +541,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -481,7 +550,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -490,19 +559,19 @@
         <v>121</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G19">
         <f>B17</f>
         <v>121</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I21">
         <f>G19/G22+B35</f>
         <v>668.00454545454545</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -515,7 +584,7 @@
         <v>60.362811791383216</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -523,7 +592,7 @@
         <v>99.2</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -532,16 +601,16 @@
         <v>88.2</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I33">
-        <f>SUM(Sheet3!A2:A11)</f>
+        <f>SUM(Range!A2:A11)</f>
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -557,77 +626,185 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A886B39-4A3A-4433-B6F6-525BA8D5BB39}">
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
+      <c r="B2">
+        <f>A2*$F$1</f>
+        <v>0.25</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ref="C2:C12" si="0">A2+B2</f>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
+      <c r="B3">
+        <f>A3*$F$1</f>
+        <v>0.5</v>
+      </c>
+      <c r="C3">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
+      <c r="B4">
+        <f>A4*$F$1</f>
+        <v>0.75</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
+      <c r="B5">
+        <f>A5*$F$1</f>
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1">
+      <c r="B6">
+        <f>A6*$F$1</f>
+        <v>1.25</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1">
+      <c r="B7">
+        <f>A7*$F$1</f>
+        <v>1.5</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:1">
+      <c r="B8">
+        <f>A8*$F$1</f>
+        <v>1.75</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>8.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:1">
+      <c r="B9">
+        <f>A9*$F$1</f>
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:1">
+      <c r="B10">
+        <f>A10*$F$1</f>
+        <v>2.25</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>11.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12">
+      <c r="B11">
+        <f>A11*$F$1</f>
+        <v>2.5</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
         <f>SUM(A2:A11)</f>
         <v>55</v>
       </c>
+      <c r="B12" s="2">
+        <f>SUM(B2:B11)</f>
+        <v>13.75</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>68.75</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -636,21 +813,21 @@
   <dimension ref="B5:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="5" spans="2:3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5">
-        <f>Sheet1!B5</f>
+        <f>Base!B5</f>
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="2:3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Modularity + 3 visualization themes based on graph size
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\temp\excelconversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB55D8F3-57A2-42F0-8EB3-F59AE737B447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881A0605-AB2D-47C3-BAE4-8E339E917148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="15105" activeTab="1" xr2:uid="{84ABE200-A998-41AD-B65F-26DE3D1D25B2}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="15105" xr2:uid="{84ABE200-A998-41AD-B65F-26DE3D1D25B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Min værdi</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Combined</t>
   </si>
 </sst>
 </file>
@@ -156,11 +159,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -514,14 +516,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A3C5551-7AC7-47CF-9FAB-6AC729A5F45A}">
-  <dimension ref="A4:I35"/>
+  <dimension ref="A4:I36"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="25.85546875" customWidth="1"/>
     <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -617,6 +620,15 @@
       <c r="B35">
         <f>Sheet2!C11</f>
         <v>666</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36">
+        <f>I33+B35+B22</f>
+        <v>6045</v>
       </c>
     </row>
   </sheetData>
@@ -628,8 +640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A886B39-4A3A-4433-B6F6-525BA8D5BB39}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,7 +657,7 @@
       <c r="B1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
         <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -660,11 +672,11 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <f>A2*$F$1</f>
+        <f t="shared" ref="B2:B11" si="0">A2*$F$1</f>
         <v>0.25</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C12" si="0">A2+B2</f>
+        <f t="shared" ref="C2:C12" si="1">A2+B2</f>
         <v>1.25</v>
       </c>
     </row>
@@ -673,11 +685,11 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <f>A3*$F$1</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="C3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
     </row>
@@ -686,11 +698,11 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <f>A4*$F$1</f>
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.75</v>
       </c>
     </row>
@@ -699,11 +711,11 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <f>A5*$F$1</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
@@ -712,11 +724,11 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <f>A6*$F$1</f>
+        <f t="shared" si="0"/>
         <v>1.25</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.25</v>
       </c>
     </row>
@@ -725,11 +737,11 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <f>A7*$F$1</f>
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
     </row>
@@ -738,11 +750,11 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <f>A8*$F$1</f>
+        <f t="shared" si="0"/>
         <v>1.75</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
     </row>
@@ -751,11 +763,11 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <f>A9*$F$1</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
@@ -764,11 +776,11 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <f>A10*$F$1</f>
+        <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11.25</v>
       </c>
     </row>
@@ -777,11 +789,11 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <f>A11*$F$1</f>
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12.5</v>
       </c>
     </row>
@@ -795,7 +807,7 @@
         <v>13.75</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>68.75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed range name issue
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\temp\excelconversion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\dalager\1 Projects\graphedexcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881A0605-AB2D-47C3-BAE4-8E339E917148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8DDF26-3AD9-482E-A1D9-D3A88BD8472A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="15105" xr2:uid="{84ABE200-A998-41AD-B65F-26DE3D1D25B2}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="15285" xr2:uid="{84ABE200-A998-41AD-B65F-26DE3D1D25B2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Base" sheetId="1" r:id="rId1"/>
-    <sheet name="Range" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Main Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Detached " sheetId="4" r:id="rId2"/>
+    <sheet name="Range Madness" sheetId="3" r:id="rId3"/>
+    <sheet name="Another Sheet" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Min værdi</t>
   </si>
@@ -86,6 +87,9 @@
   </si>
   <si>
     <t>Combined</t>
+  </si>
+  <si>
+    <t>Range</t>
   </si>
 </sst>
 </file>
@@ -519,7 +523,7 @@
   <dimension ref="A4:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,7 +613,7 @@
         <v>10</v>
       </c>
       <c r="I33">
-        <f>SUM(Range!A2:A11)</f>
+        <f>SUM('Range Madness'!A2:A11)</f>
         <v>55</v>
       </c>
     </row>
@@ -618,7 +622,7 @@
         <v>9</v>
       </c>
       <c r="B35">
-        <f>Sheet2!C11</f>
+        <f>'Another Sheet'!C11</f>
         <v>666</v>
       </c>
     </row>
@@ -637,11 +641,69 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A62C8B0-9B26-4010-BBA9-E9962728F236}">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f>SUM(A2:A4)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>666</v>
+      </c>
+      <c r="B14">
+        <f>A14</f>
+        <v>666</v>
+      </c>
+      <c r="C14">
+        <f>B14</f>
+        <v>666</v>
+      </c>
+      <c r="D14">
+        <f>C14</f>
+        <v>666</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A886B39-4A3A-4433-B6F6-525BA8D5BB39}">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,7 +882,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ABE836A-7B38-4DD4-A533-851050ABB9CE}">
   <dimension ref="B5:C11"/>
   <sheetViews>
@@ -835,7 +897,7 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <f>Base!B5</f>
+        <f>'Main Sheet'!B5</f>
         <v>11</v>
       </c>
     </row>

</xml_diff>